<commit_message>
small changes in existing files
</commit_message>
<xml_diff>
--- a/weather_data/Weather_data_of_NJ.xlsx
+++ b/weather_data/Weather_data_of_NJ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Documents/APC 524/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Documents/APC 524/CLM/Community_Land_Model/weather_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D365E9-3A2F-7747-BE4E-059CCCF09708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6576F5-2776-E344-BA34-7EB8B084CD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="1560" windowWidth="24060" windowHeight="17260" xr2:uid="{2E91C1E1-584F-E944-9EFD-C3E8D4BDFFC9}"/>
+    <workbookView xWindow="5340" yWindow="740" windowWidth="24060" windowHeight="17220" xr2:uid="{2E91C1E1-584F-E944-9EFD-C3E8D4BDFFC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,8 +166,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A5A075-7D4E-4B4F-A64D-4CBB2887228B}">
   <dimension ref="A1:V378"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,31 +494,31 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
       <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
@@ -583,7 +583,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3">
@@ -636,7 +636,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4">
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5">
@@ -742,7 +742,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6">
@@ -795,7 +795,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7">
@@ -846,9 +846,13 @@
       <c r="Q7">
         <v>0</v>
       </c>
+      <c r="T7">
+        <f>SUM(I$3:I$1048576)/365</f>
+        <v>70.766027397260316</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8">
@@ -899,9 +903,13 @@
       <c r="Q8">
         <v>0.04</v>
       </c>
+      <c r="T8">
+        <f>_xlfn.STDEV.S(I$3:I$1048576)</f>
+        <v>16.306201100805175</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9">
@@ -952,10 +960,10 @@
       <c r="Q9">
         <v>0.16</v>
       </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10">
@@ -1006,10 +1014,10 @@
       <c r="Q10">
         <v>0</v>
       </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1060,10 +1068,10 @@
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="V11" s="4"/>
+      <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1114,10 +1122,10 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="V12" s="4"/>
+      <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1168,10 +1176,10 @@
       <c r="Q13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V13" s="4"/>
+      <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14">
@@ -1222,10 +1230,10 @@
       <c r="Q14">
         <v>0.25</v>
       </c>
-      <c r="V14" s="4"/>
+      <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1276,10 +1284,10 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="V15" s="4"/>
+      <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1330,10 +1338,10 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="V16" s="4"/>
+      <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17">
@@ -1384,10 +1392,10 @@
       <c r="Q17">
         <v>0</v>
       </c>
-      <c r="V17" s="4"/>
+      <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18">
@@ -1438,10 +1446,10 @@
       <c r="Q18">
         <v>0</v>
       </c>
-      <c r="V18" s="4"/>
+      <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19">
@@ -1492,10 +1500,10 @@
       <c r="Q19">
         <v>0</v>
       </c>
-      <c r="V19" s="4"/>
+      <c r="V19" s="3"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20">
@@ -1546,10 +1554,10 @@
       <c r="Q20">
         <v>0.03</v>
       </c>
-      <c r="V20" s="4"/>
+      <c r="V20" s="3"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21">
@@ -1600,10 +1608,10 @@
       <c r="Q21">
         <v>0.04</v>
       </c>
-      <c r="V21" s="4"/>
+      <c r="V21" s="3"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22">
@@ -1654,10 +1662,10 @@
       <c r="Q22">
         <v>0</v>
       </c>
-      <c r="V22" s="4"/>
+      <c r="V22" s="3"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23">
@@ -1708,10 +1716,10 @@
       <c r="Q23">
         <v>0</v>
       </c>
-      <c r="V23" s="4"/>
+      <c r="V23" s="3"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24">
@@ -1762,10 +1770,10 @@
       <c r="Q24">
         <v>0.12</v>
       </c>
-      <c r="V24" s="4"/>
+      <c r="V24" s="3"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25">
@@ -1816,10 +1824,10 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="V25" s="4"/>
+      <c r="V25" s="3"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26">
@@ -1870,10 +1878,10 @@
       <c r="Q26">
         <v>0</v>
       </c>
-      <c r="V26" s="4"/>
+      <c r="V26" s="3"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1926,7 +1934,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28">
@@ -1979,7 +1987,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29">
@@ -2032,7 +2040,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30">
@@ -2085,7 +2093,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31">
@@ -2138,7 +2146,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32">
@@ -2191,7 +2199,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33">

</xml_diff>